<commit_message>
chore: update sample excel file
</commit_message>
<xml_diff>
--- a/anonymised_data.xlsx
+++ b/anonymised_data.xlsx
@@ -11,55 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>S/No</t>
   </si>
   <si>
     <t>Annonymised</t>
-  </si>
-  <si>
-    <t>Pre-Intervention</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please sign and return the attached form of authority. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">I can confirm that your ID check has now been completed.  
-I hope you manage to find your driving licence.  
-Now I just need your signed form of authority and signed front page of the engagement letter please. 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The terms of business letter and engagement letter were sent to you by email on &lt;DATE&gt; August, I have attached them to this email for you again.  
-Please sign page 12 of the terms of business and the front page of the engagement letter. 
-If you have access to a printer, you can print the documents and sign them, then take a photo of the signatures on your smart phone and email this to me.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thank you for providing the signed terms of business.
-The acknowledgement you received was after you had kindly completed the &lt;ORGANIZATION&gt; check.
-Please sign and return the attached form of authority form.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I’ve now finalised the letter to the opposition.  Please read this through very carefully. You must take care to ensure this accurately reflects your views, as it may be later relied on in court. 
-If you are happy that the letter is accurate then please sign a copy and return it to me.  Sending the signed version back by email is fine. 
-Please let me know if there are any amendments you want to make.  We can discuss these if that is easier for you. 
-I look forward to hearing from you. </t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Post-Intervention</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I hope you are well.  I have received the below response from Mr M &lt;DATE&gt;.  
-If you wish for me to continue to deal with this matter once I receive the opponent’s response to your offer, I will need money on account of &lt;MONEY&gt; please. This is broken down as 2 hours at my rate of &lt;MONEY1&gt; plus VAT. 
-If the matter is settled quickly and less than 2 hours of my time is required, then we can refund any money left on account. But this of course depends on the content Mr M's response.  
-I look forward to hearing from you.  </t>
   </si>
   <si>
     <t xml:space="preserve">I hope you are well. 
@@ -81,6 +38,27 @@
     <t xml:space="preserve">Just to confirm following our telephone conversation, I have a few quick questions to ask you in relation to the company structure.  
 Thank you for agreeing to speak to me &lt;DATE&gt; at 12.15. 
 Have a lovely evening. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I have spoken with my costs team and we do not need you to sign a new &lt;ORGANIZATION&gt;. I need to make you aware however that the &lt;ORGANIZATION1&gt; included a reference to qualified one way cost shifting in the event that you were unsuccessful in the claim, this does not apply to the case and if you were to be unsuccessful, you would be liable to pay the Defendant's costs to be assessed if not agreed.
+As to my fees, these are covered by the CFA with the agreed success fee. All work is carried out at my hourly rate of &lt;MONEY&gt; plus VAT. Our costs are presently &lt;MONEY1&gt; plus VAT. I anticipate the fees to trial could exceed &lt;MONEY2&gt; plus VAT. I will update you as to the costs at various points throughout the case however they are for information only, we do not require you to pay this.</t>
+  </si>
+  <si>
+    <t>Please find attached invoice for the caveat removal.</t>
+  </si>
+  <si>
+    <t>Out conveyancing team are dealing and will be liaising with the solicitors.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It doesn’t appear that’s what they have done, their emails suggest otherwise. 
+My real concern is this will all now fall apart. If P tried to engage with T and she has refused that is one thing but if they have been contacting her to say you are dealing, then she is right to say no. It’s difficult to say without sight of their paperwork.  
+She can request your mums bank details to make payment but you need to know how much she has so would will need to speak with her to ensure all beneficiaries paid and she doesn’t keep the money which was the whole point in agreeing an independent solicitor. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sometimes technology is great, sometimes not. 
+I can do &lt;DATE&gt; morning in our Walker House &lt;ORGANIZATION1&gt; 10-1 or &lt;DATE1&gt; &lt;DATE2&gt; or 1-3 in our &lt;ORGANIZATION&gt; office. 
+Please let me know if either of these work or I can ask my IT team to set up a 3 way call, I am unable to do it directly from my mobile. 
+In the meantime, I will continue my review so that when we speak, I will hopefully be able to answer some of your initial questions. </t>
   </si>
 </sst>
 </file>
@@ -461,7 +439,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B10"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -548,54 +526,6 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
feat: anonymise dates and numbers as well
</commit_message>
<xml_diff>
--- a/anonymised_data.xlsx
+++ b/anonymised_data.xlsx
@@ -11,12 +11,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>S/No</t>
   </si>
   <si>
     <t>Annonymised</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I hope you are well.  I have received the below response from Mr M &lt;DATE&gt;.  
+If you wish for me to continue to deal with this matter once I receive the opponent’s response to your offer, I will need money on account of &lt;MONEY&gt; please. This is broken down as 2 hours at my rate of &lt;MONEY1&gt; plus VAT. 
+If the matter is settled quickly and less than 2 hours of my time is required, then we can refund any money left on account. But this of course depends on the content Mr M's response.  
+I look forward to hearing from you.  </t>
   </si>
   <si>
     <t xml:space="preserve">I hope you are well. 
@@ -439,7 +445,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -526,6 +532,14 @@
         <v>10</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>